<commit_message>
Corrección de errores. Agregué la expresión regular que busca palabras que empiezan con mayúscula seguida de artículos, seguido o no de más palabras con mayúscula.
Falta implementar la expresió nregular para encontrar empresas S.A. de C.V.
</commit_message>
<xml_diff>
--- a/tablas/resultado.xlsx
+++ b/tablas/resultado.xlsx
@@ -4729,8 +4729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1033" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1056" sqref="B1056"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5261,23 +5261,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5341,43 +5341,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="E31" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="E32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregué a la regla 2 una función de similitud para corregir el problema de (Escrito).
También cambié la programación de la regla 1 para meter en un solo for
todos los casos similares.
</commit_message>
<xml_diff>
--- a/tablas/resultado.xlsx
+++ b/tablas/resultado.xlsx
@@ -4729,8 +4729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5501,23 +5501,23 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="6" t="s">
+      <c r="E39" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>102</v>
       </c>
     </row>
@@ -6038,37 +6038,37 @@
         <v>165</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="2" t="s">
+    <row r="66" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E66" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F66" s="2" t="s">
+      <c r="E66" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F66" s="9" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="2" t="s">
+    <row r="67" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F67" s="2" t="s">
+      <c r="E67" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F67" s="9" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>